<commit_message>
Meat Tenderizer HeavyAttack Done
If this needs to be edited just let me know
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53340B82-53E6-4FB4-97E9-62FE09B20A06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4A9DBA-EFF1-4DC8-9EAA-F6659916913B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +196,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -390,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -466,12 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,9 +487,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -503,6 +501,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -821,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,94 +859,94 @@
   <sheetData>
     <row r="1" spans="1:23" s="27" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="24"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="40" t="s">
         <v>38</v>
       </c>
       <c r="C1" s="25"/>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="35" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="44"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="39"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="39"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="39"/>
+      <c r="P1" s="44"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="39"/>
+      <c r="S1" s="44"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="39"/>
+      <c r="V1" s="44"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="29"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="29"/>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="29"/>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="N2" s="29"/>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="Q2" s="29"/>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="T2" s="29"/>
-      <c r="U2" s="40" t="s">
+      <c r="U2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="40" t="s">
+      <c r="V2" s="37" t="s">
         <v>30</v>
       </c>
       <c r="W2" s="29"/>
@@ -967,146 +977,146 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="41"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
       <c r="T4" s="7"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
       <c r="W4" s="7"/>
     </row>
     <row r="5" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="41"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="7"/>
       <c r="F5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="7"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="42"/>
+      <c r="J5" s="39"/>
       <c r="K5" s="7"/>
       <c r="L5" s="20"/>
-      <c r="M5" s="42"/>
+      <c r="M5" s="39"/>
       <c r="N5" s="7"/>
       <c r="O5" s="20"/>
-      <c r="P5" s="42"/>
+      <c r="P5" s="39"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="20"/>
-      <c r="S5" s="42"/>
+      <c r="S5" s="39"/>
       <c r="T5" s="7"/>
       <c r="U5" s="20"/>
-      <c r="V5" s="42"/>
+      <c r="V5" s="39"/>
       <c r="W5" s="7"/>
     </row>
     <row r="6" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="41"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="7"/>
       <c r="F6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="42"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="7"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="42"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="7"/>
       <c r="L6" s="20"/>
-      <c r="M6" s="42"/>
+      <c r="M6" s="39"/>
       <c r="N6" s="7"/>
       <c r="O6" s="20"/>
-      <c r="P6" s="42"/>
+      <c r="P6" s="39"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="20"/>
-      <c r="S6" s="42"/>
+      <c r="S6" s="39"/>
       <c r="T6" s="7"/>
       <c r="U6" s="20"/>
-      <c r="V6" s="42"/>
+      <c r="V6" s="39"/>
       <c r="W6" s="7"/>
     </row>
     <row r="7" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="41"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="7"/>
       <c r="F7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="7"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="42"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="7"/>
       <c r="L7" s="20"/>
-      <c r="M7" s="42"/>
+      <c r="M7" s="39"/>
       <c r="N7" s="7"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="42"/>
+      <c r="P7" s="39"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="20"/>
-      <c r="S7" s="42"/>
+      <c r="S7" s="39"/>
       <c r="T7" s="7"/>
       <c r="U7" s="20"/>
-      <c r="V7" s="42"/>
+      <c r="V7" s="39"/>
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="41"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="7"/>
       <c r="F8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="7"/>
       <c r="I8" s="20"/>
-      <c r="J8" s="42"/>
+      <c r="J8" s="39"/>
       <c r="K8" s="7"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="42"/>
+      <c r="M8" s="39"/>
       <c r="N8" s="7"/>
       <c r="O8" s="20"/>
-      <c r="P8" s="42"/>
+      <c r="P8" s="39"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="20"/>
-      <c r="S8" s="42"/>
+      <c r="S8" s="39"/>
       <c r="T8" s="7"/>
       <c r="U8" s="20"/>
-      <c r="V8" s="42"/>
+      <c r="V8" s="39"/>
       <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:23" s="9" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1135,10 +1145,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1146,8 +1156,8 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5"/>
@@ -1165,8 +1175,8 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="5"/>
@@ -1176,8 +1186,8 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="5"/>
@@ -1187,8 +1197,8 @@
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5"/>
@@ -1206,8 +1216,8 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="5"/>
@@ -1225,8 +1235,8 @@
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="5"/>
@@ -1236,8 +1246,8 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="5"/>
@@ -1280,10 +1290,10 @@
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="4"/>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
@@ -1291,8 +1301,8 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="5"/>
@@ -1310,8 +1320,8 @@
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36" t="s">
+      <c r="A21" s="33"/>
+      <c r="B21" s="34" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="5"/>
@@ -1329,8 +1339,8 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="5"/>
@@ -1340,8 +1350,8 @@
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="36" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="34" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="5"/>
@@ -1359,8 +1369,8 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36" t="s">
+      <c r="A24" s="33"/>
+      <c r="B24" s="34" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="5"/>
@@ -1378,8 +1388,8 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="5"/>
@@ -1389,8 +1399,8 @@
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="34" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="5"/>
@@ -1408,19 +1418,27 @@
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="45" t="s">
+        <v>8</v>
+      </c>
       <c r="E27" s="3"/>
+      <c r="F27" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="34" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="5"/>
@@ -1430,8 +1448,8 @@
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="36" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="5"/>
@@ -1441,8 +1459,8 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="5"/>
@@ -1452,8 +1470,8 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="36" t="s">
+      <c r="A31" s="33"/>
+      <c r="B31" s="34" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="5"/>
@@ -1585,15 +1603,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Meat Tenderizer Stab Anim Done
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\repo\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327AFC9A-3846-4E7D-AA75-ED146CD12843}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278EA7F2-E052-4EC5-8ECC-BB16BD77EAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -411,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -531,6 +531,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
@@ -850,7 +854,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,8 +1374,12 @@
         <v>13</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="3"/>
       <c r="K22" s="3"/>
     </row>
@@ -1419,8 +1427,12 @@
         <v>15</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="47"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="3"/>
       <c r="K25" s="3"/>
     </row>
@@ -1468,10 +1480,12 @@
         <v>19</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28"/>
-      <c r="E28" s="3"/>
-      <c r="F28"/>
-      <c r="G28"/>
+      <c r="D28" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="47"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="3"/>
       <c r="K28" s="3"/>
     </row>

</xml_diff>

<commit_message>
Dual Wield Fast Attack done
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278EA7F2-E052-4EC5-8ECC-BB16BD77EAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9C903-5114-4D91-8D59-549DE790C3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -411,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -522,6 +522,10 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -531,10 +535,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
@@ -853,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,35 +892,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="46"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="46"/>
+      <c r="J1" s="48"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="46"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="46"/>
+      <c r="P1" s="48"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="46"/>
+      <c r="S1" s="48"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="46"/>
+      <c r="V1" s="48"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -999,10 +1002,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1167,10 +1170,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="45"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1320,10 +1323,10 @@
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="45"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="4"/>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
@@ -1377,9 +1380,13 @@
       <c r="D22" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="K22" s="3"/>
     </row>
@@ -1427,12 +1434,16 @@
         <v>15</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+      <c r="D25" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="K25" s="3"/>
     </row>
@@ -1480,12 +1491,16 @@
         <v>19</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>31</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="K28" s="3"/>
     </row>

</xml_diff>

<commit_message>
updates to excell sheet
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\New repo\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9C903-5114-4D91-8D59-549DE790C3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C74B1F-B8B4-47CC-A7FE-5EBA8312B12D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -526,6 +526,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -533,9 +536,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,35 +892,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="48"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="48"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="48"/>
+      <c r="M1" s="49"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="48"/>
+      <c r="P1" s="49"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="48"/>
+      <c r="S1" s="49"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="48"/>
+      <c r="V1" s="49"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1170,10 +1170,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1205,14 +1205,14 @@
         <v>27</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="19" t="s">
-        <v>22</v>
+      <c r="D12" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="19" t="s">
+      <c r="F12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H12" s="3"/>
@@ -1224,8 +1224,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
+      <c r="D13" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="3"/>
+      <c r="F13" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="K13" s="3"/>
     </row>
@@ -1323,10 +1331,10 @@
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="47"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
@@ -1495,10 +1503,10 @@
         <v>22</v>
       </c>
       <c r="E28" s="44"/>
-      <c r="F28" s="49" t="s">
+      <c r="F28" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="49" t="s">
+      <c r="G28" s="46" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="3"/>

</xml_diff>

<commit_message>
Dual Wield Stab done
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\New repo\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C74B1F-B8B4-47CC-A7FE-5EBA8312B12D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D148F0B-177E-412F-9331-B38261BE0DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -411,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -522,13 +522,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -536,6 +529,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -856,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,35 +888,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="49"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="49"/>
+      <c r="J1" s="46"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="49"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="49"/>
+      <c r="P1" s="46"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="49"/>
+      <c r="S1" s="46"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="49"/>
+      <c r="V1" s="46"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -1002,10 +998,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1170,10 +1166,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="48"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1331,10 +1327,10 @@
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="4"/>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
@@ -1499,14 +1495,14 @@
         <v>19</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="46" t="s">
+      <c r="D28" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="47" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="3"/>

</xml_diff>

<commit_message>
added two hand idle field
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\New repo\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D148F0B-177E-412F-9331-B38261BE0DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C26BA-5D30-4BD3-B9DB-B731974A30FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="41">
   <si>
     <t>Avocado</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Production Chart</t>
+  </si>
+  <si>
+    <t>Idle Two Handed</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +273,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -411,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -522,6 +531,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -531,7 +543,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -850,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,35 +900,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="46"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="46"/>
+      <c r="J1" s="47"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="46"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="46"/>
+      <c r="P1" s="47"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="46"/>
+      <c r="S1" s="47"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="46"/>
+      <c r="V1" s="47"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -998,10 +1010,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1166,10 +1178,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1301,65 +1313,59 @@
       <c r="H17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+    </row>
+    <row r="19" spans="1:23" s="1" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="18" t="s">
-        <v>8</v>
-      </c>
+      <c r="B20" s="46"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>31</v>
-      </c>
       <c r="H20" s="3"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="34" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="18" t="s">
@@ -1378,17 +1384,17 @@
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="34" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="19" t="s">
-        <v>22</v>
+      <c r="D22" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="19" t="s">
+      <c r="F22" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H22" s="3"/>
@@ -1397,17 +1403,17 @@
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="18" t="s">
-        <v>8</v>
+      <c r="D23" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="18" t="s">
+      <c r="F23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="19" t="s">
         <v>31</v>
       </c>
       <c r="H23" s="3"/>
@@ -1416,7 +1422,7 @@
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
       <c r="B24" s="34" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="18" t="s">
@@ -1435,7 +1441,7 @@
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="33"/>
       <c r="B25" s="34" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="18" t="s">
@@ -1454,7 +1460,7 @@
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="18" t="s">
@@ -1473,10 +1479,10 @@
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="34" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3"/>
@@ -1492,17 +1498,17 @@
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="34" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="42" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="47" t="s">
+      <c r="F28" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="3"/>
@@ -1511,18 +1517,26 @@
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="17"/>
+      <c r="D29" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="E29" s="3"/>
+      <c r="F29" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>31</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
       <c r="B30" s="34" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="17"/>
@@ -1533,7 +1547,7 @@
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
       <c r="B31" s="34" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="17"/>
@@ -1541,40 +1555,43 @@
       <c r="H31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:23" s="1" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
+    </row>
+    <row r="33" spans="1:23" s="1" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="17"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="3"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
       <c r="K33" s="3"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B34" s="13"/>
       <c r="C34" s="5"/>
       <c r="D34" s="17"/>
@@ -1582,7 +1599,7 @@
       <c r="H34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="5"/>
       <c r="D35" s="17"/>
@@ -1590,7 +1607,7 @@
       <c r="H35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="5"/>
       <c r="D36" s="17"/>
@@ -1598,7 +1615,7 @@
       <c r="H36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B37" s="13"/>
       <c r="C37" s="5"/>
       <c r="D37" s="17"/>
@@ -1606,7 +1623,7 @@
       <c r="H37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
       <c r="C38" s="5"/>
       <c r="D38" s="17"/>
@@ -1614,7 +1631,7 @@
       <c r="H38" s="3"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B39" s="13"/>
       <c r="C39" s="5"/>
       <c r="D39" s="17"/>
@@ -1622,7 +1639,7 @@
       <c r="H39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B40" s="13"/>
       <c r="C40" s="5"/>
       <c r="D40" s="17"/>
@@ -1630,7 +1647,7 @@
       <c r="H40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B41" s="13"/>
       <c r="C41" s="5"/>
       <c r="D41" s="17"/>
@@ -1638,7 +1655,7 @@
       <c r="H41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
       <c r="C42" s="5"/>
       <c r="D42" s="17"/>
@@ -1646,7 +1663,7 @@
       <c r="H42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B43" s="13"/>
       <c r="C43" s="5"/>
       <c r="D43" s="17"/>
@@ -1654,7 +1671,7 @@
       <c r="H43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B44" s="13"/>
       <c r="C44" s="5"/>
       <c r="D44" s="17"/>
@@ -1662,9 +1679,17 @@
       <c r="H44" s="3"/>
       <c r="K44" s="3"/>
     </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="13"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="K45" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>

</xml_diff>

<commit_message>
Heavy Dual Wield Attack Done
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\New repo\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C26BA-5D30-4BD3-B9DB-B731974A30FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B3B71-EB9C-4CD4-8F39-7A7D9A0E2ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>Avocado</t>
   </si>
@@ -534,6 +534,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -541,9 +544,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,35 +900,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="47"/>
+      <c r="J1" s="48"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="47"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="47"/>
+      <c r="P1" s="48"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="47"/>
+      <c r="S1" s="48"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="47"/>
+      <c r="V1" s="48"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -1010,10 +1010,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1178,10 +1178,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="46"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1319,10 +1319,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="48"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -1352,10 +1352,10 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="46"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
@@ -1406,14 +1406,14 @@
         <v>13</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="19" t="s">
-        <v>22</v>
+      <c r="D23" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="19" t="s">
+      <c r="F23" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H23" s="3"/>

</xml_diff>

<commit_message>
One Handed Block Anim in Progress
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B3B71-EB9C-4CD4-8F39-7A7D9A0E2ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A0654-CD19-49DE-BF75-C58BEF96B1E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>Avocado</t>
   </si>
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -544,6 +544,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:G23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,8 +1542,16 @@
         <v>20</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="17"/>
+      <c r="D30" s="49" t="s">
+        <v>22</v>
+      </c>
       <c r="E30" s="3"/>
+      <c r="F30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="K30" s="3"/>
     </row>

</xml_diff>

<commit_message>
One Handed Block Done
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A0654-CD19-49DE-BF75-C58BEF96B1E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C590A5DC-C39B-44BF-927A-2CED85784A68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
   <si>
     <t>Avocado</t>
   </si>
@@ -537,6 +537,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -544,9 +547,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -868,7 +868,7 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F31" sqref="F31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,35 +903,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="48"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="48"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="48"/>
+      <c r="M1" s="49"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="48"/>
+      <c r="P1" s="49"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="48"/>
+      <c r="S1" s="49"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="48"/>
+      <c r="V1" s="49"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -1013,10 +1013,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1181,10 +1181,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1355,10 +1355,10 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
@@ -1542,14 +1542,14 @@
         <v>20</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="49" t="s">
-        <v>22</v>
+      <c r="D30" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="19" t="s">
+      <c r="F30" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H30" s="3"/>
@@ -1561,8 +1561,16 @@
         <v>26</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="17"/>
+      <c r="D31" s="46" t="s">
+        <v>22</v>
+      </c>
       <c r="E31" s="3"/>
+      <c r="F31" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="K31" s="3"/>
     </row>

</xml_diff>

<commit_message>
Working on Two Handed Block
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\repo\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0334960-3E42-42D2-A48B-F0391A635D4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D79294-7FFD-454E-8CAD-5BD9AD3A728B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>Avocado</t>
   </si>
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -535,9 +535,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -867,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,35 +900,35 @@
         <v>32</v>
       </c>
       <c r="E1" s="25"/>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="49"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="49"/>
+      <c r="J1" s="48"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="49"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="26"/>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="49"/>
+      <c r="P1" s="48"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="49"/>
+      <c r="S1" s="48"/>
       <c r="T1" s="26"/>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="49"/>
+      <c r="V1" s="48"/>
       <c r="W1" s="25"/>
     </row>
     <row r="2" spans="1:23" s="30" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -1013,10 +1010,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="7"/>
       <c r="D4" s="38"/>
       <c r="E4" s="7"/>
@@ -1181,10 +1178,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="48"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1363,10 +1360,10 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="48"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
@@ -1569,14 +1566,14 @@
         <v>26</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="46" t="s">
-        <v>22</v>
+      <c r="D31" s="42" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="19" t="s">
+      <c r="F31" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H31" s="3"/>

</xml_diff>

<commit_message>
Blueberry and Chili Model done
Still need rigging, also made model specific folders so animation folder isn't so crowded
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHTI\Desktop\repo\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989CA71-7160-4D24-8DA5-D616FDFB8F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A15D5D-EE7C-4683-863D-205747A7F63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
+    <workbookView xWindow="-75" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -523,6 +523,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -843,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1034,9 @@
       <c r="I5" s="19"/>
       <c r="J5" s="38"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="19"/>
+      <c r="L5" s="47" t="s">
+        <v>8</v>
+      </c>
       <c r="M5" s="38"/>
       <c r="N5" s="7"/>
       <c r="O5" s="19"/>
@@ -1040,7 +1045,9 @@
       <c r="R5" s="19"/>
       <c r="S5" s="38"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="19"/>
+      <c r="U5" s="47" t="s">
+        <v>8</v>
+      </c>
       <c r="V5" s="38"/>
       <c r="W5" s="7"/>
     </row>

</xml_diff>

<commit_message>
Broccoli Modelled, Minor changes to Blue and Chili
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A15D5D-EE7C-4683-863D-205747A7F63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712E6B86-83DB-46A2-BE11-5F6D3F1ED9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
+    <workbookView xWindow="0" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -516,6 +516,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -523,9 +526,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,35 +882,35 @@
         <v>31</v>
       </c>
       <c r="E1" s="24"/>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="46"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="24"/>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="46"/>
+      <c r="J1" s="47"/>
       <c r="K1" s="24"/>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="46"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="25"/>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="46"/>
+      <c r="P1" s="47"/>
       <c r="Q1" s="25"/>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="46"/>
+      <c r="S1" s="47"/>
       <c r="T1" s="25"/>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="46"/>
+      <c r="V1" s="47"/>
       <c r="W1" s="24"/>
     </row>
     <row r="2" spans="1:23" s="29" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -992,10 +992,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="7"/>
       <c r="D4" s="37"/>
       <c r="E4" s="7"/>
@@ -1034,18 +1034,20 @@
       <c r="I5" s="19"/>
       <c r="J5" s="38"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="44" t="s">
         <v>8</v>
       </c>
       <c r="M5" s="38"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="19"/>
+      <c r="O5" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="P5" s="38"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="19"/>
       <c r="S5" s="38"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="47" t="s">
+      <c r="U5" s="44" t="s">
         <v>8</v>
       </c>
       <c r="V5" s="38"/>
@@ -1164,10 +1166,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="45"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1352,10 +1354,10 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="45"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>

</xml_diff>

<commit_message>
Uploaded Blueberry and Tofu Rigged Models
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miranda\Documents\GitHub\Capstone2020_SliceNDice\ArtBible\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REPOS\Capstone2020\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10440583-7EA6-4559-A972-F86A4BC9387E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C49C987-8AC6-406A-90CD-0100F0FCA5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
   <si>
     <t>Avocado</t>
   </si>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1031,9 @@
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="19"/>
+      <c r="I5" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="J5" s="38"/>
       <c r="K5" s="7"/>
       <c r="L5" s="44" t="s">
@@ -1068,7 +1070,9 @@
       </c>
       <c r="G6" s="38"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="J6" s="38"/>
       <c r="K6" s="7"/>
       <c r="L6" s="44" t="s">
@@ -1105,7 +1109,9 @@
       </c>
       <c r="G7" s="38"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="J7" s="38"/>
       <c r="K7" s="7"/>
       <c r="L7" s="44" t="s">
@@ -1123,7 +1129,9 @@
       </c>
       <c r="S7" s="38"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="19"/>
+      <c r="U7" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="V7" s="38"/>
       <c r="W7" s="7"/>
     </row>

</xml_diff>

<commit_message>
updated excell anim sheet
</commit_message>
<xml_diff>
--- a/ArtBible/Animations.xlsx
+++ b/ArtBible/Animations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REPOS\Capstone2020\Capstone2020_SliceNDice\ArtBible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C49C987-8AC6-406A-90CD-0100F0FCA5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B58DD9-EC28-421E-B45C-33AE5FD21520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{171624AE-FEA1-4F9D-8CDA-95F81799CECB}"/>
   </bookViews>
@@ -216,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +264,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -405,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -510,9 +516,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,6 +529,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -846,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C87541-A194-4104-88A4-86EE4C4B95A9}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,35 +901,35 @@
         <v>31</v>
       </c>
       <c r="E1" s="24"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="24"/>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="47"/>
+      <c r="J1" s="46"/>
       <c r="K1" s="24"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="47"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="25"/>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="47"/>
+      <c r="P1" s="46"/>
       <c r="Q1" s="25"/>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="47"/>
+      <c r="S1" s="46"/>
       <c r="T1" s="25"/>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="47"/>
+      <c r="V1" s="46"/>
       <c r="W1" s="24"/>
     </row>
     <row r="2" spans="1:23" s="29" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -992,10 +1011,10 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="7"/>
       <c r="D4" s="37"/>
       <c r="E4" s="7"/>
@@ -1031,27 +1050,27 @@
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="38"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="M5" s="38"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="P5" s="38"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="44" t="s">
+      <c r="R5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="S5" s="38"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="V5" s="38"/>
@@ -1070,27 +1089,27 @@
       </c>
       <c r="G6" s="38"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="38"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="M6" s="38"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="P6" s="38"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="44" t="s">
+      <c r="R6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="S6" s="38"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="44" t="s">
+      <c r="U6" s="43" t="s">
         <v>8</v>
       </c>
       <c r="V6" s="38"/>
@@ -1109,27 +1128,27 @@
       </c>
       <c r="G7" s="38"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="38"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="M7" s="38"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="44" t="s">
+      <c r="O7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="38"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="44" t="s">
+      <c r="R7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="S7" s="38"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="44" t="s">
+      <c r="U7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="V7" s="38"/>
@@ -1190,10 +1209,10 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="46"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="4"/>
       <c r="D10" s="17"/>
       <c r="E10" s="3"/>
@@ -1257,62 +1276,104 @@
       <c r="H13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33" t="s">
+    <row r="14" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="48"/>
+      <c r="B14" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="51"/>
+      <c r="F14" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33" t="s">
+      <c r="H14" s="51"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+    </row>
+    <row r="15" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="48"/>
+      <c r="B15" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="42" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33" t="s">
+      <c r="H15" s="51"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+    </row>
+    <row r="16" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="48"/>
+      <c r="B16" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="18" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="51"/>
+      <c r="F16" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
@@ -1378,10 +1439,10 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="46"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
@@ -1546,75 +1607,117 @@
         <v>19</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="42" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="43" t="s">
+      <c r="F29" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="42" t="s">
         <v>30</v>
       </c>
       <c r="H29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33" t="s">
+    <row r="30" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="48"/>
+      <c r="B30" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="18" t="s">
+      <c r="C30" s="49"/>
+      <c r="D30" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="51"/>
+      <c r="F30" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="33" t="s">
+      <c r="H30" s="51"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+    </row>
+    <row r="31" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="48"/>
+      <c r="B31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="18" t="s">
+      <c r="C31" s="49"/>
+      <c r="D31" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="51"/>
+      <c r="F31" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33" t="s">
+      <c r="H31" s="51"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+    </row>
+    <row r="32" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="48"/>
+      <c r="B32" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="18" t="s">
+      <c r="C32" s="49"/>
+      <c r="D32" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="51"/>
+      <c r="F32" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="50"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="50"/>
     </row>
     <row r="33" spans="1:23" s="1" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>

</xml_diff>